<commit_message>
All modalities done + Late fusion 91% Acc
</commit_message>
<xml_diff>
--- a/AI & Models/Text/preprocessed_train.xlsx
+++ b/AI & Models/Text/preprocessed_train.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,10 +436,15 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>text</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>label</t>
         </is>
@@ -448,960 +453,1455 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>either barrel stick certain like going kill im lost justifing second valley saying thought shooting back</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+          <t>trial_lie_045</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>know quote responsible chrs share holder dataset available completely locked statement responsible quote lawabiding chr completely anecdotal therefore conjecture</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>far detail every detail sometimes general sense ’ going sometimes ’ far fog go ’ word spoken screamed yelled processing sort thing physical thing remember feel physically remember feel internally emotionally well ’ word spoken meaning remember feel make sense</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+          <t>trial_lie_048</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>used f word several time okay im sorry let rephrase made mentioned f word towards several time</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>asked instinctively going drive anyway right said going stay going pick said yes personal connection grandfather killed drunk driver whenever come anyone intoxicated could possibility driving like going go anywhere moment making sure going stay vicinity asked said yes</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
+          <t>trial_lie_005</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>told ammm … trying figure stuff ammm … asked like … mean never forget smoking cigarette like really calm looked said would say said … told laura dead like know like … basically told ammm … night laura come house died whenever left panicked freaked got … started freaking asking didnt call cop stutter … call help like told going told ammm … got scared black man dead white woman nobody gon na believe accident</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>brother sister childreni know fun loving uncle im cant continue experience thing life kid certainly way explain make sense situation im truly sorry</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+          <t>trial_lie_056</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>yes believe er abusive relationship yes um certainly putting friend family um destruction property seems minimal point um change victim personality</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>yeah maybe three month business struggling well even thinking quitting point alexander flown town guest speaker solid city market attended training inspired kind changed business around encounter personally kept going much better</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
+          <t>trial_lie_027</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>lunging gun going sort contemporanios ’ remember close happened exactly moment one right happened fast seemed happen would say far distance maybe far mr babbikey sp court reporter ’ say sure absolute certainty</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>’ think often cause usually call would texting computer gmail kind see contact ’ actually online think one point wrote ‘ hi text ’ online responded back started kind talking way</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
+          <t>trial_truth_004</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>uh office got call uh maybe close nine clock dont remember somewhere eight nine rusty said uh someone side house sort completely coherent said someone like sleeping side house called police oh go really quickly talk police ended calling back told whole story happened um put ian car every day around time ians car seat right passenger side back walked around smelled gas um walked cause sort exit garage little bit get side car smelled gas uh gas meter pipe side left side house youre looking front walked spot near air conditioner said man lying facedown ground</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>trial_truth_013</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>assumption ’ long time ago ’ know six month ago two year ago really ’ know yeah ’ try pry much relationship felt like yeah ’ know long</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>mean pop right upon screen got gmail open somebody say know hi pop right reply also carry conversation thing mean ’ kind like text message back forth ’ immediate responding right away sometimes even responding thing 2 3 question away know</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
+          <t>trial_lie_011</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>uh cruise husband hadnt vacation year alone without child pause clear throat project needed complete hemy insisted completed day way required input way finish work night</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>talked everybody know know flirtatious mean ah know um dont know ’ know told ’ know enough knew flirt know remember clancy telling know time know know would flirt everybody goofing around nobody really took seriously</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
+          <t>trial_truth_048</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>um tanbark started notice debris road way noticed uhhh tire mark wasnt exactly exactly sure debris ahhh started following noticed damaged roadway ahh looked saw white car tree</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>um tanbark started notice debris road way noticed uhhh tire mark wasnt exactly exactly sure debris ahhh started following noticed damaged roadway ahh looked saw white car tree</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
+          <t>trial_lie_019</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>well cant happened fast initially think run went hallway right got hallway door shut seemed like obstacle would give time catch open door way run around door equal distance open could run way thought initially run door around something create distance last time run route successful running room</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>um whenever little um oldest nephew um two year younger always close whenever really little spent lot time whenever um freshman high school went lived</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
+          <t>trial_lie_012</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>dont know maybe ten nine thirty ten something along line might even slightly later</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>pushed face definitely face pushed dont know purpose scratched neck scratched neck erra rag tshirt anyway id taking care house tore shirt</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
+          <t>trial_lie_037</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>straddled hit started choking couldnt breath umm airway cut couldnt breath umm head hurting really bad felt like head gon na explode</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>statement ive never alone candace conte never molested candace conte mean think told never ive never okay get right ive never alone candace conte ever never alone candace conte</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
+          <t>trial_truth_030</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>started investigation similarly start um investigation uh whats called primary briefing assisting uh detective uh criminalistics detective scientific portion investigation well um member command staff everyones present representative omi district attorney office uh get everybody together um particular instance many u uh inside garage uh alexander fixtons house present briefing allowed u use uh garage uh thats started investigation um briefed officer scene could get lay land figure kind uh know summary happened</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>gon na go forward know nothing crime</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
+          <t>trial_truth_058</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>um whenever little um oldest nephew um two year younger always close whenever really little spent lot time whenever um freshman high school went lived</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>werethey taller table therein walk way umwe staring placelooking aroundtaking picture insideoutsidecapture much possible uh kind stopped uh started talking uh um two girl two guy drinking trying uhto say something none made sense um telling amazed many picture takenand stuff uh said really understandable</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
+          <t>trial_lie_001</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>sir absolutely sir sir</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>tactical officer already scene deployed inner perimeter already um officer purdue already deployed highground position next two walked officer perez officer ramon hernelez walked going send individual officer weimerskirtz requesting additional manpower</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
+          <t>trial_truth_029</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>yes kitchen getting ready light heard little bloop bloop back um garbage turned somebody ringing doorbell blood dripping head screaming theyd shot</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>knew get kid back ’ wan na look got gun get kid back ’ flail little bit get back police come shot boy gone say … well could ’ look round wanted kill someone could ’ trying kill nobody ’ hostage young folk scared see man made testify folk going jail ’ come say nothing oh ’ mad understand scared ’ like people like make like see make gone make testify made</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
+          <t>trial_truth_044</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>um remember going basement remember like young lady um fell kitchen intoxicated ’ walk um staff one staff member actually made comment um ’ time remember seeing</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>correction arent made system gon na happen someone know trust gon na happen dont want dont want anywhone go family go went hell back nobody country suffer like ill best make sure gon na happen anyone else</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
+          <t>trial_truth_005</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>rusty backed garage rusty communication know hemy never responded spoken im sure rusty would recognized stayed silent entire time rusty panicked got car backed driveway end driveway picking phone dial 911 hemy ran across lawn place someone stalking house month would known existed</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>um person congregation involved activity like elder would sit individual try determine whats going objective jesus said hundred sheep one lost leave ninetynine go find one objective help individual whether er er worshiping er someone anything like celebrate christmas fornication whatever happens elder would mate individual based person um attitude time direct relevance</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
+          <t>trial_lie_046</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>first time remember mr miller washaving kinda like argument officer moving people area toward street could uh block uh sidewalk uh aggressive officer didnt understand needed everybody follow order wanted everybodys safety mean give order step street</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>didnt really know well saw couple time really wasnt placing face address didnt talk anybody lived would go school come home uh</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
+          <t>trial_truth_010</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>yeah maybe three month business struggling well even thinking quitting point alexander flown town guest speaker solid city market attended training inspired kind changed business around encounter personally kept going much better</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ahhh didnt go dance club drinking activity know time dance club got</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
+          <t>trial_lie_013</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ah dont remember evidently tried call hemy probably tell left office w something happened seemed normal thing done tell bos left office something happened husband</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>ah dont remember evidently tried call hemy probably tell left office w something happened seemed normal thing done tell bos left office something happened husband</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
+          <t>trial_lie_016</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>well recall filled gas can rather loose gas hose somewhere didnt anywhere put um hung hung end transaction thats probably could know mean could put back trunk whatever started car vise versa um one point didnt want ground hung ended transaction ’ probably one maybe topping gas tank another</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>um remember going basement remember like young lady um fell kitchen intoxicated ’ walk um staff one staff member actually made comment um ’ time remember seeing</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
+          <t>trial_truth_055</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>nothing typically see case like um childhood drug alcoholism molestation thing like none thing occurred family um dont know guess would sort joke mom didnt beat hard enough dont really mitigation</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>well cant happened fast initially think run went hallway right got hallway door shut seemed like obstacle would give time catch open door way run around door equal distance open could run way thought initially run door around something create distance last time run route successful running room</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>1</v>
+          <t>trial_truth_016</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>three friend deceased standing right next testified said guy shot best friend</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>saw aa man ground inaudible bleeding back head time trying call 911and weresightransferring something like “ ’ transfer ’ transfer ” yes</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
+          <t>trial_truth_038</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>next thing remember uh coming house um pulling gun waistband telling u get effing floor uh two nolan</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>sentenced forty sixty year prision crime didnt commit trial judge exceded sentence guideline said failed show remorse told know felt terrible happen woman shoudnt happen anyone cant show remorse somethig didnt</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>0</v>
+          <t>trial_lie_025</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>far detail every detail sometimes general sense ’ going sometimes ’ far fog go ’ word spoken screamed yelled processing sort thing physical thing remember feel physically remember feel internally emotionally well ’ word spoken meaning remember feel make sense</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>lying isnt something typically im going say ive never told lie life incident lie told case tied directly back either protecting travis reputation involvement death way ashamed death also wanted edify travis good way didnt want de edify say hateful thing especially passed away also didnt want construed motive example violent</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>1</v>
+          <t>trial_truth_018</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>answered question much could knew knew nothing murder rape</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>think choking hand free torso arm free may tried push ’ want injure wanted get quick ’ last long</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
+          <t>trial_lie_023</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>lying isnt something typically im going say ive never told lie life incident lie told case tied directly back either protecting travis reputation involvement death way ashamed death also wanted edify travis good way didnt want de edify say hateful thing especially passed away also didnt want construed motive example violent</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>three friend deceased standing right next testified said guy shot best friend</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
+          <t>trial_truth_037</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>several investigator scene um executing warrant search warrant took um room house actually took um room right walk walk living room um jonathan room</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>nothing typically see case like um childhood drug alcoholism molestation thing like none thing occurred family um dont know guess would sort joke mom didnt beat hard enough dont really mitigation</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
+          <t>trial_truth_051</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>woke lot pain lot pressure sound somebody moaning quickly realized bo shut eye laid dont even think decision consciously made waited done andhe got literally picked blanket threw</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>u represented people year system get letter prisioners um family know person improperly convicted need something one el job inocence project itelse marvelously</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>0</v>
+          <t>trial_lie_031</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>well know struggled day based logic would fought dont know thing ended ended</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>told ammm … trying figure stuff ammm … asked like … mean never forget smoking cigarette like really calm looked said would say said … told laura dead like know like … basically told ammm … night laura come house died whenever left panicked freaked got … started freaking asking didnt call cop stutter … call help like told going told ammm … got scared black man dead white woman nobody gon na believe accident</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
+          <t>trial_lie_054</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>believe evidence support domestic violence yes think bias incorrect word mr martinez dont believe im biased</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>lot talk know seduced jodi frankly jodi seductive person shes pretty straightforward uhm jodi terrible jodi isnt terrible think medium nancy grace jane velez mitchell dr drew insidious sound sane</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>1</v>
+          <t>trial_truth_059</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>married two year um divorced 10 month old basically young didnt know marriage supposed know knew wanted go school jealous um really didnt want work go school even go grocery store</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>didnt instantaneous effect mr dziekanski still stapler hand uh gone cause mistaken doesnt mean lying best job could time</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
+          <t>trial_lie_010</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>idea uh work presumably work thing im ssure nope im sure work related there seem coincidental im sure something else going call talk frequently work matter there</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>umwell remember heard shot umand remember getting vehicleandi fell ground um thats spo jerry johnson heard come</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>0</v>
+          <t>trial_lie_026</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>believed ’ okay circumstance take someone life even defending life ’ believed never really stopped consider society would view someone defending felt like done something wrong afraid consequence would</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>five item first taken serology process needed determine type dna present reason sperm cell identified take process call differential separation trying separate sperm cell epithelial cell</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
+          <t>trial_truth_009</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>mean pop right upon screen got gmail open somebody say know hi pop right reply also carry conversation thing mean ’ kind like text message back forth ’ immediate responding right away sometimes even responding thing 2 3 question away know</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>said hungry get something pizza receipt siting called ordered pizza man came right tim tim guy stopped standing partially opened door tim talked gun</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
+          <t>trial_lie_029</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>go back choking incident fact body slammed standing thought trying get top even fell felt still trying get top grabbing</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>talked kind book liked read mean atlas shrugged thinking girl rich win friend influence people lot interest great conversationalist phone lot common first met shes business woman national convention entrepreneur thought attractive trait thing sounded like somebody wanted get know</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
+          <t>trial_truth_056</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>mmm initially ive never twitter dont even know look like heard people reading magazine um 2009 somebody started false twitter account name began tweeting pretending shut um became sort idea thought february decided go</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>next thing remember uh coming house um pulling gun waistband telling u get effing floor uh two nolan</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
+          <t>trial_truth_025</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>correction arent made system gon na happen someone know trust gon na happen dont want dont want anywhone go family go went hell back nobody country suffer like ill best make sure gon na happen anyone else</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>well recall filled gas can rather loose gas hose somewhere didnt anywhere put um hung hung end transaction thats probably could know mean could put back trunk whatever started car vise versa um one point didnt want ground hung ended transaction ’ probably one maybe topping gas tank another</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
+          <t>trial_lie_006</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>didnt last time saw whenever fell whenever came already bathroom never saw ever whenever got boat covered honestly didnt even know middle seat saw boat day</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>drink bar maybe one two ammm … got onto dance floor explained ammm … trained dancer time going able dance freely like release im much space got dancing alone dance floor came join dance floor ahhh … join necessarily dance floor initially also dancing ammm time reached hand … defense said twirled around ammm thats</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>1</v>
+          <t>trial_truth_008</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>fine laughing simple little thing never felt like anything wrong day felt like socially first time saw crowd thought much comfortable oneonone first time noticed little awkward social area didnt seem like talked much people people would talk wasnt jodi knew cause one one talkative insightful different</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>approached time tripped rug kind bumped heading nursery ammm know guy seen layout there ahhh loveseat right rocking chair right next there little wall whenever tripped rug bumped grant approached grabbed kind pulled pulling back telling chill started fighting whenever little wall right loveseat kicked whenever went chair landed floor went ran bedroom lily didnt even stick around see happened got bedroom little grant trying come coming door asked noise told chair fell come back bedroom ammm asked daddy told picking chair</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
+          <t>trial_lie_050</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>fist temple kept hitting spot guess head strong id like believe went doctor four day finally went back work</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>wonderful mean came ukraine always dreamed family like belcanies first adopted mom wonderful exactly dreamed perfect took ballet went school wonderful family perfect</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>0</v>
+          <t>trial_lie_017</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>took took long time took long time get point never wanted admit id written suicide letter sent note sent envelope grandmother open nov 10th 2008 hoping dead giving little time get affair order date rolled time rolled still evolution time year went gradual process began feel right keeping instead</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>fine laughing simple little thing never felt like anything wrong day felt like socially first time saw crowd thought much comfortable oneonone first time noticed little awkward social area didnt seem like talked much people people would talk wasnt jodi knew cause one one talkative insightful different</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
+          <t>trial_truth_006</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>really didnt tell anything said accident said accident ian fine accident didnt really tell screamed phone asking going said need come dropped phone ran office</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ummm started go ground first started asking question stash girl house ummm started asking name idea talking really started asking like girl house said ask three one time two time something like preceded getting u ground kind going house looking anything value didnt looking</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
+          <t>trial_truth_054</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>psychologist explained society need umm persecute people get sort gratification might something going umm beside dont really convoluted could talk hour umm</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ahhh got hotel remember ammm … sitting er … sitting briefly balcony room additional time thats youre asking besides … explained</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
+          <t>trial_lie_008</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ahhh didnt go dance club drinking activity know time dance club got</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>proceeded step back living room front fireplace william sitting love seat still sitting shock repeatedly tell get ground three u face wood floor tell u “ ’ look ’ look ” started rummaging house find stuff asked asked else house ’ say anything said “ one ”</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>0</v>
+          <t>trial_lie_044</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>none u looking three people involved uh shooting another three individual street corner</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>born durango colorado mother single mother two older sister karen berry dory gardner one older brother um quite bit younger primarily grew um lived back forth texas new mexico 6 year old point mother married step father um lived lived new mexico approximately fifth grade</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
+          <t>trial_truth_012</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>’ think often cause usually call would texting computer gmail kind see contact ’ actually online think one point wrote ‘ hi text ’ online responded back started kind talking way</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>itsits hard swallow know hadnt done anything wasnt sexual predator</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
+          <t>trial_truth_007</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>idea police officer presume youd ask mother brother nope said didnt know taken yep went house fairly catatonic state dad brother started making phone call local hospital eventually got hold dont know whatever hospital atlanta medical center wouldnt tell dad anything taken got car left thats correct yes instructed best idea keep day care uh donna woman run day care yep thats safest place uh</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>lunging gun going sort contemporanios ’ remember close happened exactly moment one right happened fast seemed happen would say far distance maybe far mr babbikey sp court reporter ’ say sure absolute certainty</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
+          <t>trial_lie_028</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>well happened fast ’ time think everything happened um seemed split second really ’ ’ time think go way way happened without really thinking best move make</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>reforming criminal justice system matter law legitimacy people respect law need believe law treat everyone um equally um fairly</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>0</v>
+          <t>trial_lie_020</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>sort came fog realized oh crap something bad happened scared call authority point</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>sir absolutely sir sir</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>1</v>
+          <t>trial_truth_036</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>ummm started go ground first started asking question stash girl house ummm started asking name idea talking really started asking like girl house said ask three one time two time something like preceded getting u ground kind going house looking anything value didnt looking</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>recall screaming yelling um dont know constitutes talking saying word thing dont recall far word dont</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>1</v>
+          <t>trial_truth_041</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>um put soft body armor put um repeat offender project hard body armor uh good rifle round augmented body armor put um changed glass noticed time day changed glass um sunglass uh clear lens eye protection uh got department rifle insured department rifle taser shotgun um made sure body armor recording device</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>served twelve year texas prison life sentence ammm exonerated dna evidence real perpetrator real murderer confession</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>0</v>
+          <t>trial_lie_009</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ahhh got hotel remember ammm … sitting er … sitting briefly balcony room additional time thats youre asking besides … explained</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>felt safe b angela great aunt felt committed well um c need stability permanency safety order able heal recover clear time gabby spent angelas receiving aunt uncle</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>0</v>
+          <t>trial_lie_014</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>think choking hand free torso arm free may tried push ’ want injure wanted get quick ’ last long</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>two black male standing door looked like tee shirt basketball short yes pull two pistol brother face told u get back house get fuck ground</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
+          <t>trial_truth_024</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>sentenced forty sixty year prision crime didnt commit trial judge exceded sentence guideline said failed show remorse told know felt terrible happen woman shoudnt happen anyone cant show remorse somethig didnt</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>well happened fast ’ time think everything happened um seemed split second really ’ ’ time think go way way happened without really thinking best move make</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
+          <t>trial_lie_004</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>told dream ammm forest killed laura didnt help get rid … gon na next</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>idea uh work presumably work thing im ssure nope im sure work related there seem coincidental im sure something else going call talk frequently work matter there</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
+          <t>trial_lie_018</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>attempt talk present better image relationship downplay negative aspect like really big deal oh ’ bad kinda thing like oh yeah knew wasnt big deal um even argument oh sure rocky turmoil friend attempt present good image travis good image relationship ups down still um good term</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>first time remember mr miller washaving kinda like argument officer moving people area toward street could uh block uh sidewalk uh aggressive officer didnt understand needed everybody follow order wanted everybodys safety mean give order step street</t>
-        </is>
-      </c>
-      <c r="B60" t="n">
+          <t>trial_lie_039</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>didnt really know well saw couple time really wasnt placing face address didnt talk anybody lived would go school come home uh</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>started investigation similarly start um investigation uh whats called primary briefing assisting uh detective uh criminalistics detective scientific portion investigation well um member command staff everyones present representative omi district attorney office uh get everybody together um particular instance many u uh inside garage uh alexander fixtons house present briefing allowed u use uh garage uh thats started investigation um briefed officer scene could get lay land figure kind uh know summary happened</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
+          <t>trial_truth_033</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>two black male standing door looked like tee shirt basketball short yes pull two pistol brother face told u get back house get fuck ground</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>mmm initially ive never twitter dont even know look like heard people reading magazine um 2009 somebody started false twitter account name began tweeting pretending shut um became sort idea thought february decided go</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>0</v>
+          <t>trial_lie_007</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>drink bar maybe one two ammm … got onto dance floor explained ammm … trained dancer time going able dance freely like release im much space got dancing alone dance floor came join dance floor ahhh … join necessarily dance floor initially also dancing ammm time reached hand … defense said twirled around ammm thats</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>fist temple kept hitting spot guess head strong id like believe went doctor four day finally went back work</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>1</v>
+          <t>trial_truth_017</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>gon na go forward know nothing crime</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>believe evidence support domestic violence yes think bias incorrect word mr martinez dont believe im biased</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>1</v>
+          <t>trial_truth_045</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>um daughter ah nicole friend long time ah pretty much cause lifer class 2005 um actually taught nicole sophomore english nicole megan band together think like 7th 10th grade um excuse basketball 7th 10th band together 4th 12th</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>would take hammer hit</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>1</v>
+          <t>trial_truth_035</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>thats one pointed gun towards face said step back game get ground ahhh facial feature hair umm cornrows bernard remember cornrows slash best men eyebrow</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>yes yep stayed uh yep prob yes yes</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>0</v>
+          <t>trial_lie_055</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>lot talk know seduced jodi frankly jodi seductive person shes pretty straightforward uhm jodi terrible jodi isnt terrible think medium nancy grace jane velez mitchell dr drew insidious sound sane</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>absolutely nothing disappearance im glad um laci disappeared um called immediately wasnt immediately couple day lacis disappearance telephoned told truth married lacis disappearance didnt know point</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
+          <t>trial_lie_047</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>time called name wasnt really conversation wasnt two part conversation</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>answered question much could knew knew nothing murder rape</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
+          <t>trial_truth_057</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>born durango colorado mother single mother two older sister karen berry dory gardner one older brother um quite bit younger primarily grew um lived back forth texas new mexico 6 year old point mother married step father um lived lived new mexico approximately fifth grade</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>right shot occurred um fallen bathroom toward sink sink garbage area kind corner didnt chase moment thats struggled floor soon broke away said fing kill bitch dont remember lot whether chased couldnt say</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>1</v>
+          <t>trial_truth_019</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>served twelve year texas prison life sentence ammm exonerated dna evidence real perpetrator real murderer confession</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ahhh lot people dont value freedom gone get back like value lot</t>
-        </is>
-      </c>
-      <c r="B70" t="n">
+          <t>trial_truth_034</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>proceeded step back living room front fireplace william sitting love seat still sitting shock repeatedly tell get ground three u face wood floor tell u “ ’ look ’ look ” started rummaging house find stuff asked asked else house ’ say anything said “ one ”</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>rusty backed garage rusty communication know hemy never responded spoken im sure rusty would recognized stayed silent entire time rusty panicked got car backed driveway end driveway picking phone dial 911 hemy ran across lawn place someone stalking house month would known existed</t>
-        </is>
-      </c>
-      <c r="B71" t="n">
-        <v>0</v>
+          <t>trial_lie_042</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>found man uh secure area luggage cart chair set around uh tried thing communicate chair went flying grabbed computer desk threw um werent getting guy violence escalating</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>interviewed police mathew hood stated jamie hood called asked pick mc donalds jamie mc donalds parent jamie asked mathew take cousin tobarriss house change mathew know mathew hood jamie hood left mc donalds</t>
-        </is>
-      </c>
-      <c r="B72" t="n">
-        <v>0</v>
+          <t>trial_lie_049</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>word front would assume would said would say would assume</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>experiencing disorientation ’ thinking gosh travis ’ choked actually thought sort wandered mind wheres nepolian head thought ’ really relation event thought kinda getting bearing um ’ completely clear remember hand around neck banging head carpet tried push blacked really shortly</t>
-        </is>
-      </c>
-      <c r="B73" t="n">
-        <v>1</v>
+          <t>trial_truth_052</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>five item first taken serology process needed determine type dna present reason sperm cell identified take process call differential separation trying separate sperm cell epithelial cell</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>sir</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>1</v>
+          <t>trial_truth_015</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>talked everybody know know flirtatious mean ah know um dont know ’ know told ’ know enough knew flirt know remember clancy telling know time know know would flirt everybody goofing around nobody really took seriously</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>uh cruise husband hadnt vacation year alone without child pause clear throat project needed complete hemy insisted completed day way required input way finish work night</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>1</v>
+          <t>trial_truth_053</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>good um treated respect loved um would like degenerative disc disease neck would bring pillow bathroom put behind head neck wouldnt hurt um um would always ask know always want talk always called baby said loved used tell loved time</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>uh office got call uh maybe close nine clock dont remember somewhere eight nine rusty said uh someone side house sort completely coherent said someone like sleeping side house called police oh go really quickly talk police ended calling back told whole story happened um put ian car every day around time ians car seat right passenger side back walked around smelled gas um walked cause sort exit garage little bit get side car smelled gas uh gas meter pipe side left side house youre looking front walked spot near air conditioner said man lying facedown ground</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>0</v>
+          <t>trial_lie_060</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>statement ive never alone candace conte never molested candace conte mean think told never ive never okay get right ive never alone candace conte ever never alone candace conte</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>believed ’ okay circumstance take someone life even defending life ’ believed never really stopped consider society would view someone defending felt like done something wrong afraid consequence would</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>1</v>
+          <t>trial_truth_003</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>yes yep stayed uh yep prob yes yes</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>used f word several time okay im sorry let rephrase made mentioned f word towards several time</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>1</v>
+          <t>trial_truth_040</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>umwell remember heard shot umand remember getting vehicleandi fell ground um thats spo jerry johnson heard come</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>recollection saw pull two knife go back im im going see basically vantage point foot turning appears possibly east point looking foot im assuming turning went ground</t>
-        </is>
-      </c>
-      <c r="B79" t="n">
-        <v>0</v>
+          <t>trial_lie_038</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>trying say something couldnt talk tried push strong um could think kid telling mom dont go dont go</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>told well finally still dark finally shown flashlight um cause mentioned shed shot head could tell hair soaked blood um least one officer ah arrived butterfly creek ah figured actual incident happened bernardino rest officer ah went residence</t>
-        </is>
-      </c>
-      <c r="B80" t="n">
-        <v>0</v>
+          <t>trial_lie_030</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>sense correct remember dropping knife screaming memory came much later um go blank dont remember putting gun car dont remember putting rope car crystal clear pretty pretty solid memory disposing go car obviously ’ remember placing car</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>really didnt tell anything said accident said accident ian fine accident didnt really tell screamed phone asking going said need come dropped phone ran office</t>
-        </is>
-      </c>
-      <c r="B81" t="n">
+          <t>trial_truth_047</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>asked instinctively going drive anyway right said going stay going pick said yes personal connection grandfather killed drunk driver whenever come anyone intoxicated could possibility driving like going go anywhere moment making sure going stay vicinity asked said yes</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>name marvin l anderson um born genova virginia um 1982 went trial convicted two count rape sodomy robery abduction um sentenced total sentence two hundred ten year spent 15 year prision five year parole exonerated two thousand</t>
-        </is>
-      </c>
-      <c r="B82" t="n">
-        <v>0</v>
+          <t>trial_lie_002</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>approached time tripped rug kind bumped heading nursery ammm know guy seen layout there ahhh loveseat right rocking chair right next there little wall whenever tripped rug bumped grant approached grabbed kind pulled pulling back telling chill started fighting whenever little wall right loveseat kicked whenever went chair landed floor went ran bedroom lily didnt even stick around see happened got bedroom little grant trying come coming door asked noise told chair fell come back bedroom ammm asked daddy told picking chair</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>conversation jodi telling talked girl even supposed together might mean</t>
-        </is>
-      </c>
-      <c r="B83" t="n">
-        <v>0</v>
+          <t>trial_lie_053</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>either barrel stick certain like going kill im lost justifing second valley saying thought shooting back</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>time called name wasnt really conversation wasnt two part conversation</t>
-        </is>
-      </c>
-      <c r="B84" t="n">
+          <t>trial_lie_022</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>well think good memory june 4th anomaly like said yesterday class cant explain kind state mind um day entire blank little piece come back many cant explain day alone put day day memory issue different average person</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>back believe ask hm asked battery take time battery charge wont able use box time thats asked would like one corded</t>
-        </is>
-      </c>
-      <c r="B85" t="n">
-        <v>0</v>
+          <t>trial_lie_003</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>sir</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>word front would assume would said would say would assume</t>
-        </is>
-      </c>
-      <c r="B86" t="n">
+          <t>trial_lie_024</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>experiencing disorientation ’ thinking gosh travis ’ choked actually thought sort wandered mind wheres nepolian head thought ’ really relation event thought kinda getting bearing um ’ completely clear remember hand around neck banging head carpet tried push blacked really shortly</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>yes believe er abusive relationship yes um certainly putting friend family um destruction property seems minimal point um change victim personality</t>
-        </is>
-      </c>
-      <c r="B87" t="n">
-        <v>1</v>
+          <t>trial_truth_043</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>tactical officer already scene deployed inner perimeter already um officer purdue already deployed highground position next two walked officer perez officer ramon hernelez walked going send individual officer weimerskirtz requesting additional manpower</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>idea police officer presume youd ask mother brother nope said didnt know taken yep went house fairly catatonic state dad brother started making phone call local hospital eventually got hold dont know whatever hospital atlanta medical center wouldnt tell dad anything taken got car left thats correct yes instructed best idea keep day care uh donna woman run day care yep thats safest place uh</t>
-        </is>
-      </c>
-      <c r="B88" t="n">
+          <t>trial_truth_049</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>felt safe b angela great aunt felt committed well um c need stability permanency safety order able heal recover clear time gabby spent angelas receiving aunt uncle</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>attempt talk present better image relationship downplay negative aspect like really big deal oh ’ bad kinda thing like oh yeah knew wasnt big deal um even argument oh sure rocky turmoil friend attempt present good image travis good image relationship ups down still um good term</t>
-        </is>
-      </c>
-      <c r="B89" t="n">
-        <v>1</v>
+          <t>trial_truth_014</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>conversation jodi telling talked girl even supposed together might mean</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>none u looking three people involved uh shooting another three individual street corner</t>
-        </is>
-      </c>
-      <c r="B90" t="n">
-        <v>1</v>
+          <t>trial_truth_060</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>yes um reginald would like long talk one long talk um late night u two guess put vulnerable position um slept together</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>woke lot pain lot pressure sound somebody moaning quickly realized bo shut eye laid dont even think decision consciously made waited done andhe got literally picked blanket threw</t>
-        </is>
-      </c>
-      <c r="B91" t="n">
-        <v>0</v>
+          <t>trial_lie_021</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>recall screaming yelling um dont know constitutes talking saying word thing dont recall far word dont</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>several investigator scene um executing warrant search warrant took um room house actually took um room right walk walk living room um jonathan room</t>
-        </is>
-      </c>
-      <c r="B92" t="n">
-        <v>0</v>
+          <t>trial_lie_061</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>oh thats word agains mine isnt think heard since become biggest inaudible well would like think thats juge isnt mean thats god</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>go back choking incident fact body slammed standing thought trying get top even fell felt still trying get top grabbing</t>
-        </is>
-      </c>
-      <c r="B93" t="n">
-        <v>1</v>
+          <t>trial_truth_011</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>talked kind book liked read mean atlas shrugged thinking girl rich win friend influence people lot interest great conversationalist phone lot common first met shes business woman national convention entrepreneur thought attractive trait thing sounded like somebody wanted get know</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>oh thats word agains mine isnt think heard since become biggest inaudible well would like think thats juge isnt mean thats god</t>
-        </is>
-      </c>
-      <c r="B94" t="n">
-        <v>1</v>
+          <t>trial_truth_046</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>werethey taller table therein walk way umwe staring placelooking aroundtaking picture insideoutsidecapture much possible uh kind stopped uh started talking uh um two girl two guy drinking trying uhto say something none made sense um telling amazed many picture takenand stuff uh said really understandable</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>thats one pointed gun towards face said step back game get ground ahhh facial feature hair umm cornrows bernard remember cornrows slash best men eyebrow</t>
-        </is>
-      </c>
-      <c r="B95" t="n">
-        <v>0</v>
+          <t>trial_lie_015</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>right shot occurred um fallen bathroom toward sink sink garbage area kind corner didnt chase moment thats struggled floor soon broke away said fing kill bitch dont remember lot whether chased couldnt say</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>took took long time took long time get point never wanted admit id written suicide letter sent note sent envelope grandmother open nov 10th 2008 hoping dead giving little time get affair order date rolled time rolled still evolution time year went gradual process began feel right keeping instead</t>
-        </is>
-      </c>
-      <c r="B96" t="n">
-        <v>1</v>
+          <t>trial_truth_032</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>told well finally still dark finally shown flashlight um cause mentioned shed shot head could tell hair soaked blood um least one officer ah arrived butterfly creek ah figured actual incident happened bernardino rest officer ah went residence</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>married two year um divorced 10 month old basically young didnt know marriage supposed know knew wanted go school jealous um really didnt want work go school even go grocery store</t>
-        </is>
-      </c>
-      <c r="B97" t="n">
+          <t>trial_lie_052</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>absolutely nothing disappearance im glad um laci disappeared um called immediately wasnt immediately couple day lacis disappearance telephoned told truth married lacis disappearance didnt know point</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>trial_truth_042</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>recollection saw pull two knife go back im im going see basically vantage point foot turning appears possibly east point looking foot im assuming turning went ground</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>